<commit_message>
implemented code base of multi_shrna_screening_ap009.ipynb
</commit_message>
<xml_diff>
--- a/data/sample description.xlsx
+++ b/data/sample description.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bli/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bli/Documents/Projects/Multi_shRNA_screening_AP009/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CD973C-5FC8-694B-9EF0-36E7F656EC8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFACD5F9-E3DA-2348-839C-E3DE70E8D225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17660" yWindow="-21100" windowWidth="34840" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="72">
   <si>
     <t>Sample ID</t>
   </si>
@@ -255,6 +255,21 @@
   </si>
   <si>
     <t>should tech rep be in group 2?</t>
+  </si>
+  <si>
+    <t>Tx</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Vehicle</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -360,7 +375,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -407,13 +422,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -440,7 +466,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -667,7 +696,7 @@
   <dimension ref="A1:Q1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -704,7 +733,9 @@
       <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="15" t="s">
+        <v>67</v>
+      </c>
       <c r="G2" s="14" t="s">
         <v>55</v>
       </c>
@@ -743,6 +774,9 @@
       <c r="E3" s="11" t="s">
         <v>54</v>
       </c>
+      <c r="F3" s="13" t="s">
+        <v>68</v>
+      </c>
       <c r="G3" s="13">
         <v>5</v>
       </c>
@@ -772,6 +806,9 @@
       <c r="E4" s="11" t="s">
         <v>54</v>
       </c>
+      <c r="F4" s="13" t="s">
+        <v>68</v>
+      </c>
       <c r="G4" s="13">
         <v>5</v>
       </c>
@@ -801,6 +838,9 @@
       <c r="E5" s="11" t="s">
         <v>54</v>
       </c>
+      <c r="F5" s="16" t="s">
+        <v>69</v>
+      </c>
       <c r="G5" s="13">
         <v>4</v>
       </c>
@@ -810,7 +850,7 @@
       <c r="I5">
         <v>2</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="J5" s="13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -830,6 +870,9 @@
       <c r="E6" s="11" t="s">
         <v>54</v>
       </c>
+      <c r="F6" s="16" t="s">
+        <v>69</v>
+      </c>
       <c r="G6" s="13">
         <v>4</v>
       </c>
@@ -839,7 +882,7 @@
       <c r="I6">
         <v>1</v>
       </c>
-      <c r="J6" s="15" t="s">
+      <c r="J6" s="13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -859,6 +902,9 @@
       <c r="E7" s="11" t="s">
         <v>54</v>
       </c>
+      <c r="F7" s="16" t="s">
+        <v>70</v>
+      </c>
       <c r="G7" s="13">
         <v>2</v>
       </c>
@@ -868,7 +914,7 @@
       <c r="I7">
         <v>2</v>
       </c>
-      <c r="J7" s="15" t="s">
+      <c r="J7" s="13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -888,6 +934,9 @@
       <c r="E8" s="11" t="s">
         <v>54</v>
       </c>
+      <c r="F8" s="16" t="s">
+        <v>70</v>
+      </c>
       <c r="G8" s="13">
         <v>2</v>
       </c>
@@ -897,7 +946,7 @@
       <c r="I8">
         <v>1</v>
       </c>
-      <c r="J8" s="15" t="s">
+      <c r="J8" s="13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -917,6 +966,9 @@
       <c r="E9" s="11" t="s">
         <v>54</v>
       </c>
+      <c r="F9" s="16" t="s">
+        <v>68</v>
+      </c>
       <c r="G9" s="13">
         <v>5</v>
       </c>
@@ -926,7 +978,7 @@
       <c r="I9">
         <v>2</v>
       </c>
-      <c r="J9" s="15" t="s">
+      <c r="J9" s="13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -946,6 +998,9 @@
       <c r="E10" s="11" t="s">
         <v>54</v>
       </c>
+      <c r="F10" s="16" t="s">
+        <v>68</v>
+      </c>
       <c r="G10" s="13">
         <v>5</v>
       </c>
@@ -955,7 +1010,7 @@
       <c r="I10">
         <v>1</v>
       </c>
-      <c r="J10" s="15" t="s">
+      <c r="J10" s="13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -975,6 +1030,9 @@
       <c r="E11" s="11" t="s">
         <v>54</v>
       </c>
+      <c r="F11" s="16" t="s">
+        <v>69</v>
+      </c>
       <c r="G11" s="13">
         <v>4</v>
       </c>
@@ -984,7 +1042,7 @@
       <c r="I11">
         <v>2</v>
       </c>
-      <c r="J11" s="15" t="s">
+      <c r="J11" s="13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1004,6 +1062,9 @@
       <c r="E12" s="11" t="s">
         <v>54</v>
       </c>
+      <c r="F12" s="16" t="s">
+        <v>69</v>
+      </c>
       <c r="G12" s="13">
         <v>4</v>
       </c>
@@ -1013,7 +1074,7 @@
       <c r="I12">
         <v>1</v>
       </c>
-      <c r="J12" s="15" t="s">
+      <c r="J12" s="13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1033,6 +1094,9 @@
       <c r="E13" s="11" t="s">
         <v>54</v>
       </c>
+      <c r="F13" s="16" t="s">
+        <v>70</v>
+      </c>
       <c r="G13" s="13">
         <v>2</v>
       </c>
@@ -1042,7 +1106,7 @@
       <c r="I13">
         <v>2</v>
       </c>
-      <c r="J13" s="15" t="s">
+      <c r="J13" s="13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1062,6 +1126,9 @@
       <c r="E14" s="11" t="s">
         <v>54</v>
       </c>
+      <c r="F14" s="16" t="s">
+        <v>70</v>
+      </c>
       <c r="G14" s="13">
         <v>2</v>
       </c>
@@ -1071,7 +1138,7 @@
       <c r="I14">
         <v>1</v>
       </c>
-      <c r="J14" s="15" t="s">
+      <c r="J14" s="13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1091,6 +1158,9 @@
       <c r="E15" s="11" t="s">
         <v>54</v>
       </c>
+      <c r="F15" s="16" t="s">
+        <v>68</v>
+      </c>
       <c r="G15" s="13">
         <v>5</v>
       </c>
@@ -1100,7 +1170,7 @@
       <c r="I15">
         <v>2</v>
       </c>
-      <c r="J15" s="15" t="s">
+      <c r="J15" s="13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1120,6 +1190,9 @@
       <c r="E16" s="11" t="s">
         <v>54</v>
       </c>
+      <c r="F16" s="16" t="s">
+        <v>68</v>
+      </c>
       <c r="G16" s="13">
         <v>5</v>
       </c>
@@ -1129,7 +1202,7 @@
       <c r="I16">
         <v>1</v>
       </c>
-      <c r="J16" s="15" t="s">
+      <c r="J16" s="13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1149,6 +1222,9 @@
       <c r="E17" s="11" t="s">
         <v>54</v>
       </c>
+      <c r="F17" s="16" t="s">
+        <v>69</v>
+      </c>
       <c r="G17" s="13">
         <v>4</v>
       </c>
@@ -1158,7 +1234,7 @@
       <c r="I17">
         <v>2</v>
       </c>
-      <c r="J17" s="15" t="s">
+      <c r="J17" s="13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1178,6 +1254,9 @@
       <c r="E18" s="11" t="s">
         <v>54</v>
       </c>
+      <c r="F18" s="16" t="s">
+        <v>69</v>
+      </c>
       <c r="G18" s="13">
         <v>4</v>
       </c>
@@ -1187,7 +1266,7 @@
       <c r="I18">
         <v>1</v>
       </c>
-      <c r="J18" s="15" t="s">
+      <c r="J18" s="13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1207,6 +1286,9 @@
       <c r="E19" s="11" t="s">
         <v>54</v>
       </c>
+      <c r="F19" s="16" t="s">
+        <v>71</v>
+      </c>
       <c r="G19" s="13">
         <v>1</v>
       </c>
@@ -1216,7 +1298,7 @@
       <c r="I19">
         <v>2</v>
       </c>
-      <c r="J19" s="15" t="s">
+      <c r="J19" s="13" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1236,6 +1318,9 @@
       <c r="E20" s="11" t="s">
         <v>54</v>
       </c>
+      <c r="F20" s="16" t="s">
+        <v>71</v>
+      </c>
       <c r="G20" s="13">
         <v>1</v>
       </c>
@@ -1245,7 +1330,7 @@
       <c r="I20" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="J20" s="15" t="s">
+      <c r="J20" s="13" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1265,6 +1350,9 @@
       <c r="E21" s="11" t="s">
         <v>54</v>
       </c>
+      <c r="F21" s="16" t="s">
+        <v>71</v>
+      </c>
       <c r="G21" s="13">
         <v>1</v>
       </c>
@@ -1274,7 +1362,7 @@
       <c r="I21" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="J21" s="15" t="s">
+      <c r="J21" s="13" t="s">
         <v>62</v>
       </c>
       <c r="K21" s="13" t="s">
@@ -1297,6 +1385,9 @@
       <c r="E22" s="11" t="s">
         <v>54</v>
       </c>
+      <c r="F22" s="16" t="s">
+        <v>70</v>
+      </c>
       <c r="G22">
         <v>2</v>
       </c>
@@ -1306,7 +1397,7 @@
       <c r="I22" s="13">
         <v>2</v>
       </c>
-      <c r="J22" s="15" t="s">
+      <c r="J22" s="13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1326,6 +1417,9 @@
       <c r="E23" s="11" t="s">
         <v>54</v>
       </c>
+      <c r="F23" s="16" t="s">
+        <v>70</v>
+      </c>
       <c r="G23">
         <v>2</v>
       </c>
@@ -1335,7 +1429,7 @@
       <c r="I23" s="13">
         <v>1</v>
       </c>
-      <c r="J23" s="15" t="s">
+      <c r="J23" s="13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1355,6 +1449,9 @@
       <c r="E24" s="11" t="s">
         <v>54</v>
       </c>
+      <c r="F24" s="16" t="s">
+        <v>71</v>
+      </c>
       <c r="G24" s="13" t="s">
         <v>63</v>
       </c>
@@ -1364,7 +1461,7 @@
       <c r="I24" s="13">
         <v>2</v>
       </c>
-      <c r="J24" s="15" t="s">
+      <c r="J24" s="13" t="s">
         <v>61</v>
       </c>
       <c r="K24" s="13" t="s">
@@ -1387,6 +1484,9 @@
       <c r="E25" s="11" t="s">
         <v>54</v>
       </c>
+      <c r="F25" s="16" t="s">
+        <v>71</v>
+      </c>
       <c r="G25" s="13" t="s">
         <v>63</v>
       </c>
@@ -1396,7 +1496,7 @@
       <c r="I25" s="13">
         <v>2</v>
       </c>
-      <c r="J25" s="15" t="s">
+      <c r="J25" s="13" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1416,6 +1516,9 @@
       <c r="E26" s="11" t="s">
         <v>54</v>
       </c>
+      <c r="F26" s="16" t="s">
+        <v>71</v>
+      </c>
       <c r="G26" s="13" t="s">
         <v>63</v>
       </c>
@@ -1425,7 +1528,7 @@
       <c r="I26" s="13">
         <v>1</v>
       </c>
-      <c r="J26" s="15" t="s">
+      <c r="J26" s="13" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>